<commit_message>
feat: Add Web Store to Excel file to scrape from
</commit_message>
<xml_diff>
--- a/src/main/resources/static/WebStores.xlsx
+++ b/src/main/resources/static/WebStores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eigenaar\IdeaProjects\cheapclothes_BackEnd\src\main\resources\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eigenaar\IdeaProjects\ProductScraper\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B7CFA0-C958-4CC7-9807-99A6A15A704A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA24C5E-6406-490C-93E5-1BB23586C1CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D6D307C0-10D5-4C8C-9EC2-A69EE4233B6B}"/>
+    <workbookView xWindow="14303" yWindow="-5033" windowWidth="28995" windowHeight="15946" xr2:uid="{D6D307C0-10D5-4C8C-9EC2-A69EE4233B6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Brand</t>
   </si>
@@ -74,9 +74,6 @@
     <t>.price-standard</t>
   </si>
   <si>
-    <t>https://www.wefashion.nl/nl_NL/sale/women/?pmin=1%2C00&amp;pmax=10%2C00&amp;srule=General%20sorting%20rule</t>
-  </si>
-  <si>
     <t>.search-result-items</t>
   </si>
   <si>
@@ -98,19 +95,64 @@
     <t>`</t>
   </si>
   <si>
-    <t>https://www.isawitfirst.com/collections/sale?page=1&amp;fct_FSM_price=1%3A10</t>
-  </si>
-  <si>
-    <t>.product-name</t>
-  </si>
-  <si>
-    <t>.view__img--1:src</t>
-  </si>
-  <si>
     <t>FALSE</t>
   </si>
   <si>
-    <t>Nasty gal</t>
+    <t>https://www.wefashion.nl/nl_NL/outlet/men</t>
+  </si>
+  <si>
+    <t>Free people</t>
+  </si>
+  <si>
+    <t>.c-pwa-product-tile</t>
+  </si>
+  <si>
+    <t>.c-pwa-product-price__current</t>
+  </si>
+  <si>
+    <t>.c-pwa-product-price__original</t>
+  </si>
+  <si>
+    <t>.c-pwa-product-tile__link</t>
+  </si>
+  <si>
+    <t>.c-pwa-image-viewer__img:src</t>
+  </si>
+  <si>
+    <t>https://www.freepeople.com/sale-all/?currency=EUR</t>
+  </si>
+  <si>
+    <t>.c-pwa-product-meta-heading</t>
+  </si>
+  <si>
+    <t>.c-pwa-tile-view-outer</t>
+  </si>
+  <si>
+    <t>Forever21</t>
+  </si>
+  <si>
+    <t>.product-grid</t>
+  </si>
+  <si>
+    <t>.product-tile</t>
+  </si>
+  <si>
+    <t>.product-tile__anchor</t>
+  </si>
+  <si>
+    <t>.pdp__name</t>
+  </si>
+  <si>
+    <t>.price__default--discount</t>
+  </si>
+  <si>
+    <t>https://www.forever21.com/us/shop/catalog/category/21men/mens-sale</t>
+  </si>
+  <si>
+    <t>.price__original &gt; .value</t>
+  </si>
+  <si>
+    <t>.product-gallery__img:src</t>
   </si>
 </sst>
 </file>
@@ -475,20 +517,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE637F-6994-4815-AE6B-64A17FF482E1}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="186.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="96.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -522,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -530,13 +572,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -545,48 +587,80 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -594,15 +668,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{2460F340-A5BE-4EDA-8B83-5E9300109318}"/>
     <hyperlink ref="I3" r:id="rId2" xr:uid="{80E8BEF2-4F9A-4BDB-95A3-DC5B043CC9CE}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{A3F55201-9F71-4049-BE58-A39ACB965A0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>